<commit_message>
Private Agents self links
</commit_message>
<xml_diff>
--- a/module-dependency-tree.xlsx
+++ b/module-dependency-tree.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igor.antonacci/src/terraform-gcp-dcos-fork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4466117-2640-8B49-8AD0-25638AF2EEF2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCA2BB9-99D8-9A4C-B7A4-3942F7450001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" xr2:uid="{6D581D0F-79C0-AC49-A1F4-765766BF3F95}"/>
   </bookViews>
@@ -573,8 +573,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7B8320E5-0314-EB47-8B52-09E4B84FAE04}">
   <dimension ref="A5:E26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="C4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -583,7 +583,7 @@
     <col min="2" max="2" width="84.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="51.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="77.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="64.33203125" customWidth="1"/>
+    <col min="5" max="5" width="78.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
[ADD] Base Cluster network name
</commit_message>
<xml_diff>
--- a/module-dependency-tree.xlsx
+++ b/module-dependency-tree.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10913"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/igor.antonacci/src/terraform-gcp-dcos-fork/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDCA2BB9-99D8-9A4C-B7A4-3942F7450001}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8238D486-C1DF-8E46-B133-4C2ED66A5940}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="20080" xr2:uid="{6D581D0F-79C0-AC49-A1F4-765766BF3F95}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="52">
   <si>
     <t>Module name</t>
   </si>
@@ -186,6 +186,9 @@
   </si>
   <si>
     <t>https://github.com/igor-antonacci-jr/terraform-gcp-compute-forwarding-rule-public-agents</t>
+  </si>
+  <si>
+    <t>https://github.com/igor-antonacci-jr/terraform-gcp-network</t>
   </si>
 </sst>
 </file>
@@ -574,7 +577,7 @@
   <dimension ref="A5:E26"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="C4" zoomScale="140" zoomScaleNormal="140" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -730,6 +733,9 @@
       </c>
       <c r="D14" s="1" t="s">
         <v>32</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -934,6 +940,7 @@
     <hyperlink ref="E7" r:id="rId33" xr:uid="{A664CEE0-F2A0-B14C-8CE1-FC3C6458C2DB}"/>
     <hyperlink ref="E17" r:id="rId34" xr:uid="{CD0E1986-25A9-5548-B368-D65AEDE10686}"/>
     <hyperlink ref="E19" r:id="rId35" xr:uid="{3CE171AB-1AD9-204B-833F-AAFC7AD6E417}"/>
+    <hyperlink ref="E14" r:id="rId36" xr:uid="{54A64D08-9548-1C40-85C6-98EEF12CC85D}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>